<commit_message>
updated iteration 2 exercise solutions
</commit_message>
<xml_diff>
--- a/FVA.xlsx
+++ b/FVA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_AD4DB114E44117BA4C33AC9DB956D708693EDF29" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7813877E-FE52-4780-B5C9-4C556E884522}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_AD4DB114E44117BA4C33AC9DB956D708693EDF29" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D6BC288C-D877-467C-A80F-B4841FDB95C2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Methode / Verfahren</t>
   </si>
   <si>
     <t>Mean Absolute Error (CV)</t>
-  </si>
-  <si>
-    <t>Forecast Value Added</t>
   </si>
   <si>
     <r>
@@ -58,19 +55,29 @@
     <t>Exponential Smoothing</t>
   </si>
   <si>
-    <t>Lineare Regression</t>
-  </si>
-  <si>
     <t>Random Forest</t>
   </si>
   <si>
-    <t>Random Forest + weitere Merkmale</t>
-  </si>
-  <si>
-    <t>Forecast Value Added %</t>
-  </si>
-  <si>
-    <t>Random Forest + weitere Merkmale + Merkmalsauswahl</t>
+    <t>FVA vs. 
+Naive Forecast</t>
+  </si>
+  <si>
+    <t>FVA vs.
+Expontential Smoothing</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FVA vs.
+Linear Regression </t>
+  </si>
+  <si>
+    <t>Random Forest mit weiteren Merkmalen</t>
+  </si>
+  <si>
+    <t>FVA vs.
+Random Forest</t>
   </si>
 </sst>
 </file>
@@ -135,11 +142,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -420,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,114 +446,122 @@
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>1056.83</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
+        <v>918.06</v>
+      </c>
+      <c r="C3" s="5">
+        <f>($B$2-B3)/$B$2</f>
+        <v>0.13130777892376255</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>504.96</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:C6" si="0">($B$2-B4)/$B$2</f>
+        <v>0.52219373030667182</v>
+      </c>
+      <c r="D4" s="5">
+        <f>($B$3-B4)/$B$3</f>
+        <v>0.44997059015750601</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>918.06</v>
-      </c>
-      <c r="C3" s="1">
-        <f>$B$2-B3</f>
-        <v>138.76999999999998</v>
-      </c>
-      <c r="D3" s="2">
-        <f>C3/$B$2</f>
-        <v>0.13130777892376255</v>
-      </c>
+      <c r="B5" s="6">
+        <v>477.2</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54846096344729045</v>
+      </c>
+      <c r="D5" s="5">
+        <f>($B$3-B5)/$B$3</f>
+        <v>0.48020826525499422</v>
+      </c>
+      <c r="E5" s="5">
+        <f>($B$4-B5)/$B$4</f>
+        <v>5.4974651457541178E-2</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>504.96</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C4:C7" si="0">$B$2-B4</f>
-        <v>551.86999999999989</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4:D7" si="1">C4/$B$2</f>
-        <v>0.52219373030667182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>472.95</v>
-      </c>
-      <c r="C5" s="1">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8">
+        <v>402.16</v>
+      </c>
+      <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>583.87999999999988</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.55248242385246438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>413.32</v>
-      </c>
-      <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>643.51</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="1"/>
-        <v>0.60890587890199943</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>413.22</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>643.6099999999999</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.60900050149976814</v>
+        <v>0.6194657608129972</v>
+      </c>
+      <c r="D6" s="5">
+        <f>($B$3-B6)/$B$3</f>
+        <v>0.56194584231967393</v>
+      </c>
+      <c r="E6" s="5">
+        <f>($B$4-B6)/$B$4</f>
+        <v>0.20358048162230663</v>
+      </c>
+      <c r="F6" s="5">
+        <f>(B5-B6)/B5</f>
+        <v>0.15725062866722542</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>